<commit_message>
* Bugfix to wildcard sets. * Updated test_compare_rule_equals. * Implemented additional compare logic in compare_engine.
</commit_message>
<xml_diff>
--- a/tests/test_artifacts/test_compare_rule_equals/test.xlsx
+++ b/tests/test_artifacts/test_compare_rule_equals/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\i-beg-to-differ\tests\test_artifacts\test_core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\i-beg-to-differ\tests\test_artifacts\test_compare_rule_equals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CE4A4-02B0-4EED-A56B-483C4F075D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68910198-6326-4572-AA59-105F3373E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7104" yWindow="2424" windowWidth="23040" windowHeight="12660" xr2:uid="{E0987C40-DE28-48BA-BC2C-209A11D1EF12}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{E0987C40-DE28-48BA-BC2C-209A11D1EF12}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>pk1</t>
   </si>
@@ -57,12 +57,6 @@
     <t>171eadc6-bd02-4648-ae29-610644a96833</t>
   </si>
   <si>
-    <t>2eb86e3a-3239-440b-8e9f-7ab13604494d</t>
-  </si>
-  <si>
-    <t>5434643f-0598-4c31-833d-d759fdc14e84</t>
-  </si>
-  <si>
     <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
   </si>
   <si>
-    <t>45346d72-b355-48c8-94ed-a907a91c4375</t>
-  </si>
-  <si>
-    <t>b15f70be-cd58-47e1-9fe6-44d7dbadb279</t>
-  </si>
-  <si>
     <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
   </si>
   <si>
@@ -115,12 +103,6 @@
   </si>
   <si>
     <t>departure</t>
-  </si>
-  <si>
-    <t>satellite</t>
-  </si>
-  <si>
-    <t>deficiency</t>
   </si>
   <si>
     <t>depressed</t>
@@ -490,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A586C3B-4F06-4978-8C06-485BAFD49602}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,16 +502,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>7.4127384735807968</v>
+        <v>7.4127384740000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -537,16 +519,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>3.1097419535443795</v>
+        <v>3.109741954</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -554,16 +536,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>9</v>
       </c>
       <c r="E4">
-        <v>10.497180630266294</v>
+        <v>10.497180630000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -571,16 +553,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>7.9065868521777345</v>
+        <v>7.9065868520000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -588,16 +570,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>8.2886376058927969</v>
+        <v>8.288637606</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -605,16 +587,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>10.457065481556475</v>
+        <v>10.457065480000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -622,16 +604,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>3.8482210167506947</v>
+        <v>8.2641600059999991</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -639,50 +621,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>0.33985071739382744</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>8.2641600064017613</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>8.1822368578921321</v>
+        <v>8.1822368579999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>